<commit_message>
Added the text extraction and merging files, including the main.py
</commit_message>
<xml_diff>
--- a/Data/images.xlsx
+++ b/Data/images.xlsx
@@ -6543,7 +6543,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B385"/>
+  <dimension ref="A1:C385"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6562,6 +6562,11 @@
           <t>Images</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Image Path</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -6569,6 +6574,11 @@
           <t>38601</t>
         </is>
       </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Data/images/38601.png</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -6576,6 +6586,11 @@
           <t>83317</t>
         </is>
       </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Data/images/83317.png</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -6583,6 +6598,11 @@
           <t>90734</t>
         </is>
       </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Data/images/90734.png</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -6590,6 +6610,11 @@
           <t>90735</t>
         </is>
       </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Data/images/90735.png</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -6597,6 +6622,11 @@
           <t>91354</t>
         </is>
       </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Data/images/91354.png</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -6616,6 +6646,11 @@
           <t>91944</t>
         </is>
       </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Data/images/91944.png</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -6623,6 +6658,11 @@
           <t>102223</t>
         </is>
       </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Data/images/102223.png</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -6678,6 +6718,11 @@
           <t>111442</t>
         </is>
       </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Data/images/111442.png</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -6685,6 +6730,11 @@
           <t>111827</t>
         </is>
       </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Data/images/111827.png</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -6692,6 +6742,11 @@
           <t>112108</t>
         </is>
       </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Data/images/112108.png</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -6723,6 +6778,11 @@
           <t>114020</t>
         </is>
       </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Data/images/114020.png</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -6730,6 +6790,11 @@
           <t>115224</t>
         </is>
       </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Data/images/115224.png</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -6737,6 +6802,11 @@
           <t>116441</t>
         </is>
       </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Data/images/116441.png</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -6744,6 +6814,11 @@
           <t>117782</t>
         </is>
       </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Data/images/117782.png</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -6751,6 +6826,11 @@
           <t>118710</t>
         </is>
       </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Data/images/118710.png</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -6842,6 +6922,11 @@
           <t>119132</t>
         </is>
       </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Data/images/119132.png</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -6849,6 +6934,11 @@
           <t>119450</t>
         </is>
       </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Data/images/119450.png</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -6856,6 +6946,11 @@
           <t>120066</t>
         </is>
       </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Data/images/120066.png</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -6887,6 +6982,11 @@
           <t>120940</t>
         </is>
       </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Data/images/120940.png</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -6894,6 +6994,11 @@
           <t>121516</t>
         </is>
       </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Data/images/121516.png</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -6901,6 +7006,11 @@
           <t>121771</t>
         </is>
       </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Data/images/121771.png</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -6908,6 +7018,11 @@
           <t>122617</t>
         </is>
       </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Data/images/122617.png</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -6915,6 +7030,11 @@
           <t>123504</t>
         </is>
       </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Data/images/123504.png</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -6922,6 +7042,11 @@
           <t>123716</t>
         </is>
       </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Data/images/123716.png</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -6989,6 +7114,11 @@
           <t>124382</t>
         </is>
       </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Data/images/124382.png</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -6996,6 +7126,11 @@
           <t>124441</t>
         </is>
       </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Data/images/124441.png</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -7027,6 +7162,11 @@
           <t>124512</t>
         </is>
       </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Data/images/124512.png</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -7034,6 +7174,11 @@
           <t>124543</t>
         </is>
       </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Data/images/124543.png</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -7041,6 +7186,11 @@
           <t>124767</t>
         </is>
       </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Data/images/124767.png</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -7048,6 +7198,11 @@
           <t>125135</t>
         </is>
       </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Data/images/125135.png</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -7103,6 +7258,11 @@
           <t>126098</t>
         </is>
       </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Data/images/126098.png</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -7110,6 +7270,11 @@
           <t>126326</t>
         </is>
       </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Data/images/126326.png</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -7117,6 +7282,11 @@
           <t>126414</t>
         </is>
       </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Data/images/126414.png</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -7124,6 +7294,11 @@
           <t>126480</t>
         </is>
       </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Data/images/126480.png</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -7131,6 +7306,11 @@
           <t>126552</t>
         </is>
       </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Data/images/126552.png</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -7138,6 +7318,11 @@
           <t>126629</t>
         </is>
       </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Data/images/126629.png</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -7145,6 +7330,11 @@
           <t>126687</t>
         </is>
       </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Data/images/126687.png</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -7152,6 +7342,11 @@
           <t>126898</t>
         </is>
       </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Data/images/126898.png</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -7159,6 +7354,11 @@
           <t>126899</t>
         </is>
       </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Data/images/126899.png</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -7166,6 +7366,11 @@
           <t>126900</t>
         </is>
       </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Data/images/126900.png</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -7233,6 +7438,11 @@
           <t>127180</t>
         </is>
       </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Data/images/127180.png</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -7240,6 +7450,11 @@
           <t>127197</t>
         </is>
       </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Data/images/127197.png</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -7259,6 +7474,11 @@
           <t>127367</t>
         </is>
       </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Data/images/127367.png</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -7266,6 +7486,11 @@
           <t>127369</t>
         </is>
       </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Data/images/127369.png</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -7273,6 +7498,11 @@
           <t>127370</t>
         </is>
       </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Data/images/127370.png</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -7316,6 +7546,11 @@
           <t>127431</t>
         </is>
       </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Data/images/127431.png</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -7323,6 +7558,11 @@
           <t>127435</t>
         </is>
       </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Data/images/127435.png</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -7330,6 +7570,11 @@
           <t>127460</t>
         </is>
       </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Data/images/127460.png</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -7385,6 +7630,11 @@
           <t>127734</t>
         </is>
       </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Data/images/127734.png</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -7392,6 +7642,11 @@
           <t>127735</t>
         </is>
       </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Data/images/127735.png</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -7399,6 +7654,11 @@
           <t>127757</t>
         </is>
       </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Data/images/127757.png</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -7406,6 +7666,11 @@
           <t>127758</t>
         </is>
       </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Data/images/127758.png</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -7413,6 +7678,11 @@
           <t>127759</t>
         </is>
       </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Data/images/127759.png</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -7420,6 +7690,11 @@
           <t>127779</t>
         </is>
       </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Data/images/127779.png</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -7427,6 +7702,11 @@
           <t>127780</t>
         </is>
       </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Data/images/127780.png</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -7434,6 +7714,11 @@
           <t>127781</t>
         </is>
       </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Data/images/127781.png</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -7441,6 +7726,11 @@
           <t>127845</t>
         </is>
       </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Data/images/127845.png</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -7496,6 +7786,11 @@
           <t>127956</t>
         </is>
       </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Data/images/127956.png</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -7503,6 +7798,11 @@
           <t>128132</t>
         </is>
       </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Data/images/128132.png</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -7510,6 +7810,11 @@
           <t>128133</t>
         </is>
       </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Data/images/128133.png</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -7577,6 +7882,11 @@
           <t>128522</t>
         </is>
       </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Data/images/128522.png</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -7584,6 +7894,11 @@
           <t>128523</t>
         </is>
       </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Data/images/128523.png</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -7591,6 +7906,11 @@
           <t>128524</t>
         </is>
       </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Data/images/128524.png</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -7622,6 +7942,11 @@
           <t>128612</t>
         </is>
       </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>Data/images/128612.png</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -7629,6 +7954,11 @@
           <t>128630</t>
         </is>
       </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Data/images/128630.png</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -7636,6 +7966,11 @@
           <t>128636</t>
         </is>
       </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Data/images/128636.png</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -7643,6 +7978,11 @@
           <t>128640</t>
         </is>
       </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>Data/images/128640.png</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -7662,6 +8002,11 @@
           <t>128793</t>
         </is>
       </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Data/images/128793.png</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -7669,6 +8014,11 @@
           <t>128795</t>
         </is>
       </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>Data/images/128795.png</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -7676,6 +8026,11 @@
           <t>128819</t>
         </is>
       </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>Data/images/128819.png</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -7683,6 +8038,11 @@
           <t>128831</t>
         </is>
       </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>Data/images/128831.png</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -7714,6 +8074,11 @@
           <t>129033</t>
         </is>
       </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>Data/images/129033.png</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -7721,6 +8086,11 @@
           <t>129049</t>
         </is>
       </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>Data/images/129049.png</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -7728,6 +8098,11 @@
           <t>129050</t>
         </is>
       </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>Data/images/129050.png</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -7735,6 +8110,11 @@
           <t>129077</t>
         </is>
       </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>Data/images/129077.png</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -7742,6 +8122,11 @@
           <t>129078</t>
         </is>
       </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>Data/images/129078.png</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -7749,6 +8134,11 @@
           <t>129131</t>
         </is>
       </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>Data/images/129131.png</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -7756,6 +8146,11 @@
           <t>129143</t>
         </is>
       </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>Data/images/129143.png</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -7763,6 +8158,11 @@
           <t>129148</t>
         </is>
       </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>Data/images/129148.png</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -7770,6 +8170,11 @@
           <t>129149</t>
         </is>
       </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>Data/images/129149.png</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -7801,6 +8206,11 @@
           <t>129201</t>
         </is>
       </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>Data/images/129201.png</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -7808,6 +8218,11 @@
           <t>129217</t>
         </is>
       </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>Data/images/129217.png</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -7815,6 +8230,11 @@
           <t>129242</t>
         </is>
       </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>Data/images/129242.png</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -7822,6 +8242,11 @@
           <t>129286</t>
         </is>
       </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>Data/images/129286.png</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -7829,6 +8254,11 @@
           <t>129317</t>
         </is>
       </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>Data/images/129317.png</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -7836,6 +8266,11 @@
           <t>129359</t>
         </is>
       </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>Data/images/129359.png</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -7843,6 +8278,11 @@
           <t>129385</t>
         </is>
       </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>Data/images/129385.png</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -7850,6 +8290,11 @@
           <t>129386</t>
         </is>
       </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>Data/images/129386.png</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -7857,6 +8302,11 @@
           <t>129393</t>
         </is>
       </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>Data/images/129393.png</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -7864,6 +8314,11 @@
           <t>129400</t>
         </is>
       </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>Data/images/129400.png</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -7895,6 +8350,11 @@
           <t>129435</t>
         </is>
       </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>Data/images/129435.png</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -7902,6 +8362,11 @@
           <t>129502</t>
         </is>
       </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>Data/images/129502.png</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -7945,6 +8410,11 @@
           <t>129540</t>
         </is>
       </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>Data/images/129540.png</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -7952,6 +8422,11 @@
           <t>129549</t>
         </is>
       </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>Data/images/129549.png</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -7959,6 +8434,11 @@
           <t>129553</t>
         </is>
       </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>Data/images/129553.png</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -7966,6 +8446,11 @@
           <t>129631</t>
         </is>
       </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>Data/images/129631.png</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -7973,6 +8458,11 @@
           <t>129632</t>
         </is>
       </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>Data/images/129632.png</t>
+        </is>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -8004,6 +8494,11 @@
           <t>129708</t>
         </is>
       </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>Data/images/129708.png</t>
+        </is>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -8011,6 +8506,11 @@
           <t>129709</t>
         </is>
       </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>Data/images/129709.png</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -8018,6 +8518,11 @@
           <t>129717</t>
         </is>
       </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>Data/images/129717.png</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -8025,6 +8530,11 @@
           <t>129722</t>
         </is>
       </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>Data/images/129722.png</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -8032,6 +8542,11 @@
           <t>129735</t>
         </is>
       </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>Data/images/129735.png</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -8039,6 +8554,11 @@
           <t>129736</t>
         </is>
       </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>Data/images/129736.png</t>
+        </is>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -8046,6 +8566,11 @@
           <t>129740</t>
         </is>
       </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>Data/images/129740.png</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -8053,6 +8578,11 @@
           <t>129746</t>
         </is>
       </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>Data/images/129746.png</t>
+        </is>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -8060,6 +8590,11 @@
           <t>129756</t>
         </is>
       </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>Data/images/129756.png</t>
+        </is>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -8079,6 +8614,11 @@
           <t>129810</t>
         </is>
       </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>Data/images/129810.png</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -8086,6 +8626,11 @@
           <t>129847</t>
         </is>
       </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>Data/images/129847.png</t>
+        </is>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -8093,6 +8638,11 @@
           <t>129854</t>
         </is>
       </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>Data/images/129854.png</t>
+        </is>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -8100,6 +8650,11 @@
           <t>129858</t>
         </is>
       </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>Data/images/129858.png</t>
+        </is>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -8107,6 +8662,11 @@
           <t>129882</t>
         </is>
       </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>Data/images/129882.png</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -8114,6 +8674,11 @@
           <t>129913</t>
         </is>
       </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>Data/images/129913.png</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -8121,6 +8686,11 @@
           <t>129916</t>
         </is>
       </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>Data/images/129916.png</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -8128,6 +8698,11 @@
           <t>129917</t>
         </is>
       </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>Data/images/129917.png</t>
+        </is>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -8171,6 +8746,11 @@
           <t>129953</t>
         </is>
       </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>Data/images/129953.png</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -8178,6 +8758,11 @@
           <t>129954</t>
         </is>
       </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>Data/images/129954.png</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -8185,6 +8770,11 @@
           <t>129958</t>
         </is>
       </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>Data/images/129958.png</t>
+        </is>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -8216,6 +8806,11 @@
           <t>129962</t>
         </is>
       </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>Data/images/129962.png</t>
+        </is>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -8223,6 +8818,11 @@
           <t>129970</t>
         </is>
       </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>Data/images/129970.png</t>
+        </is>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -8230,6 +8830,11 @@
           <t>129972</t>
         </is>
       </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>Data/images/129972.png</t>
+        </is>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -8261,6 +8866,11 @@
           <t>129975</t>
         </is>
       </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>Data/images/129975.png</t>
+        </is>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -8268,6 +8878,11 @@
           <t>129988</t>
         </is>
       </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>Data/images/129988.png</t>
+        </is>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -8275,6 +8890,11 @@
           <t>129989</t>
         </is>
       </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>Data/images/129989.png</t>
+        </is>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -8282,6 +8902,11 @@
           <t>130002</t>
         </is>
       </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>Data/images/130002.png</t>
+        </is>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -8289,6 +8914,11 @@
           <t>130010</t>
         </is>
       </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>Data/images/130010.png</t>
+        </is>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -8296,6 +8926,11 @@
           <t>130021</t>
         </is>
       </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>Data/images/130021.png</t>
+        </is>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -8303,6 +8938,11 @@
           <t>130023</t>
         </is>
       </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>Data/images/130023.png</t>
+        </is>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -8322,6 +8962,11 @@
           <t>130048</t>
         </is>
       </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>Data/images/130048.png</t>
+        </is>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -8329,6 +8974,11 @@
           <t>130051</t>
         </is>
       </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>Data/images/130051.png</t>
+        </is>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -8336,6 +8986,11 @@
           <t>130053</t>
         </is>
       </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>Data/images/130053.png</t>
+        </is>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -8343,6 +8998,11 @@
           <t>130092</t>
         </is>
       </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>Data/images/130092.png</t>
+        </is>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -8350,6 +9010,11 @@
           <t>130093</t>
         </is>
       </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>Data/images/130093.png</t>
+        </is>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -8381,6 +9046,11 @@
           <t>130097</t>
         </is>
       </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>Data/images/130097.png</t>
+        </is>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -8388,6 +9058,11 @@
           <t>130099</t>
         </is>
       </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>Data/images/130099.png</t>
+        </is>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -8395,6 +9070,11 @@
           <t>130100</t>
         </is>
       </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>Data/images/130100.png</t>
+        </is>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -8438,6 +9118,11 @@
           <t>130116</t>
         </is>
       </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>Data/images/130116.png</t>
+        </is>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -8445,6 +9130,11 @@
           <t>130117</t>
         </is>
       </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>Data/images/130117.png</t>
+        </is>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -8452,6 +9142,11 @@
           <t>130124</t>
         </is>
       </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>Data/images/130124.png</t>
+        </is>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -8483,6 +9178,11 @@
           <t>130137</t>
         </is>
       </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>Data/images/130137.png</t>
+        </is>
+      </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
@@ -8490,6 +9190,11 @@
           <t>130146</t>
         </is>
       </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>Data/images/130146.png</t>
+        </is>
+      </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -8497,6 +9202,11 @@
           <t>130147</t>
         </is>
       </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>Data/images/130147.png</t>
+        </is>
+      </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
@@ -8504,6 +9214,11 @@
           <t>130148</t>
         </is>
       </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>Data/images/130148.png</t>
+        </is>
+      </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
@@ -8511,6 +9226,11 @@
           <t>130149</t>
         </is>
       </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>Data/images/130149.png</t>
+        </is>
+      </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
@@ -8518,6 +9238,11 @@
           <t>130155</t>
         </is>
       </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>Data/images/130155.png</t>
+        </is>
+      </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -8525,6 +9250,11 @@
           <t>130163</t>
         </is>
       </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>Data/images/130163.png</t>
+        </is>
+      </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
@@ -8532,6 +9262,11 @@
           <t>130164</t>
         </is>
       </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>Data/images/130164.png</t>
+        </is>
+      </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
@@ -8539,6 +9274,11 @@
           <t>130171</t>
         </is>
       </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>Data/images/130171.png</t>
+        </is>
+      </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
@@ -8546,6 +9286,11 @@
           <t>130177</t>
         </is>
       </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>Data/images/130177.png</t>
+        </is>
+      </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
@@ -8673,6 +9418,11 @@
           <t>130207</t>
         </is>
       </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>Data/images/130207.png</t>
+        </is>
+      </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
@@ -8680,6 +9430,11 @@
           <t>130208</t>
         </is>
       </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>Data/images/130208.png</t>
+        </is>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
@@ -8687,6 +9442,11 @@
           <t>130209</t>
         </is>
       </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>Data/images/130209.png</t>
+        </is>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
@@ -8694,6 +9454,11 @@
           <t>130211</t>
         </is>
       </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>Data/images/130211.png</t>
+        </is>
+      </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
@@ -8701,6 +9466,11 @@
           <t>130213</t>
         </is>
       </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>Data/images/130213.png</t>
+        </is>
+      </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
@@ -8708,6 +9478,11 @@
           <t>130214</t>
         </is>
       </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>Data/images/130214.png</t>
+        </is>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
@@ -8727,6 +9502,11 @@
           <t>130216</t>
         </is>
       </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>Data/images/130216.png</t>
+        </is>
+      </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
@@ -8734,6 +9514,11 @@
           <t>130239</t>
         </is>
       </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>Data/images/130239.png</t>
+        </is>
+      </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
@@ -8741,6 +9526,11 @@
           <t>130240</t>
         </is>
       </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>Data/images/130240.png</t>
+        </is>
+      </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
@@ -8748,6 +9538,11 @@
           <t>130241</t>
         </is>
       </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>Data/images/130241.png</t>
+        </is>
+      </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
@@ -8755,6 +9550,11 @@
           <t>130243</t>
         </is>
       </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>Data/images/130243.png</t>
+        </is>
+      </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
@@ -8774,6 +9574,11 @@
           <t>130250</t>
         </is>
       </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>Data/images/130250.png</t>
+        </is>
+      </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
@@ -8781,6 +9586,11 @@
           <t>130251</t>
         </is>
       </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>Data/images/130251.png</t>
+        </is>
+      </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
@@ -8788,6 +9598,11 @@
           <t>130254</t>
         </is>
       </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>Data/images/130254.png</t>
+        </is>
+      </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
@@ -8795,6 +9610,11 @@
           <t>130255</t>
         </is>
       </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>Data/images/130255.png</t>
+        </is>
+      </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
@@ -8802,6 +9622,11 @@
           <t>130256</t>
         </is>
       </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>Data/images/130256.png</t>
+        </is>
+      </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
@@ -8809,6 +9634,11 @@
           <t>130262</t>
         </is>
       </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>Data/images/130262.png</t>
+        </is>
+      </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
@@ -8816,6 +9646,11 @@
           <t>130265</t>
         </is>
       </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>Data/images/130265.png</t>
+        </is>
+      </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
@@ -8823,6 +9658,11 @@
           <t>130270</t>
         </is>
       </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>Data/images/130270.png</t>
+        </is>
+      </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
@@ -8830,6 +9670,11 @@
           <t>130283</t>
         </is>
       </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>Data/images/130283.png</t>
+        </is>
+      </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
@@ -8837,6 +9682,11 @@
           <t>130292</t>
         </is>
       </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>Data/images/130292.png</t>
+        </is>
+      </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
@@ -8844,6 +9694,11 @@
           <t>130294</t>
         </is>
       </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>Data/images/130294.png</t>
+        </is>
+      </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
@@ -8851,6 +9706,11 @@
           <t>130295</t>
         </is>
       </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>Data/images/130295.png</t>
+        </is>
+      </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
@@ -8882,6 +9742,11 @@
           <t>130300</t>
         </is>
       </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>Data/images/130300.png</t>
+        </is>
+      </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
@@ -8889,6 +9754,11 @@
           <t>130301</t>
         </is>
       </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>Data/images/130301.png</t>
+        </is>
+      </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
@@ -8896,6 +9766,11 @@
           <t>130302</t>
         </is>
       </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>Data/images/130302.png</t>
+        </is>
+      </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
@@ -8903,6 +9778,11 @@
           <t>130305</t>
         </is>
       </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>Data/images/130305.png</t>
+        </is>
+      </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
@@ -8910,6 +9790,11 @@
           <t>130306</t>
         </is>
       </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>Data/images/130306.png</t>
+        </is>
+      </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
@@ -8929,6 +9814,11 @@
           <t>130325</t>
         </is>
       </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>Data/images/130325.png</t>
+        </is>
+      </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
@@ -8936,6 +9826,11 @@
           <t>130330</t>
         </is>
       </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>Data/images/130330.png</t>
+        </is>
+      </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
@@ -8943,6 +9838,11 @@
           <t>130331</t>
         </is>
       </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>Data/images/130331.png</t>
+        </is>
+      </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
@@ -8950,6 +9850,11 @@
           <t>130336</t>
         </is>
       </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>Data/images/130336.png</t>
+        </is>
+      </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
@@ -8957,6 +9862,11 @@
           <t>130339</t>
         </is>
       </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>Data/images/130339.png</t>
+        </is>
+      </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
@@ -9000,6 +9910,11 @@
           <t>130354</t>
         </is>
       </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>Data/images/130354.png</t>
+        </is>
+      </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
@@ -9007,6 +9922,11 @@
           <t>130373</t>
         </is>
       </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>Data/images/130373.png</t>
+        </is>
+      </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
@@ -9014,6 +9934,11 @@
           <t>130395</t>
         </is>
       </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>Data/images/130395.png</t>
+        </is>
+      </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
@@ -9021,6 +9946,11 @@
           <t>130396</t>
         </is>
       </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>Data/images/130396.png</t>
+        </is>
+      </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
@@ -9052,6 +9982,11 @@
           <t>130413</t>
         </is>
       </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>Data/images/130413.png</t>
+        </is>
+      </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
@@ -9071,6 +10006,11 @@
           <t>130424</t>
         </is>
       </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>Data/images/130424.png</t>
+        </is>
+      </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
@@ -9078,6 +10018,11 @@
           <t>130432</t>
         </is>
       </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>Data/images/130432.png</t>
+        </is>
+      </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
@@ -9085,6 +10030,11 @@
           <t>130433</t>
         </is>
       </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>Data/images/130433.png</t>
+        </is>
+      </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
@@ -9092,6 +10042,11 @@
           <t>130435</t>
         </is>
       </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>Data/images/130435.png</t>
+        </is>
+      </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
@@ -9099,6 +10054,11 @@
           <t>130436</t>
         </is>
       </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>Data/images/130436.png</t>
+        </is>
+      </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
@@ -9106,6 +10066,11 @@
           <t>130437</t>
         </is>
       </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>Data/images/130437.png</t>
+        </is>
+      </c>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
@@ -9113,6 +10078,11 @@
           <t>130438</t>
         </is>
       </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>Data/images/130438.png</t>
+        </is>
+      </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
@@ -9120,6 +10090,11 @@
           <t>130439</t>
         </is>
       </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>Data/images/130439.png</t>
+        </is>
+      </c>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
@@ -9127,6 +10102,11 @@
           <t>130440</t>
         </is>
       </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>Data/images/130440.png</t>
+        </is>
+      </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
@@ -9134,6 +10114,11 @@
           <t>130441</t>
         </is>
       </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>Data/images/130441.png</t>
+        </is>
+      </c>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
@@ -9141,6 +10126,11 @@
           <t>130442</t>
         </is>
       </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>Data/images/130442.png</t>
+        </is>
+      </c>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
@@ -9148,6 +10138,11 @@
           <t>130443</t>
         </is>
       </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>Data/images/130443.png</t>
+        </is>
+      </c>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
@@ -9155,6 +10150,11 @@
           <t>130454</t>
         </is>
       </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>Data/images/130454.png</t>
+        </is>
+      </c>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
@@ -9174,6 +10174,11 @@
           <t>130487</t>
         </is>
       </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>Data/images/130487.png</t>
+        </is>
+      </c>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
@@ -9181,6 +10186,11 @@
           <t>130498</t>
         </is>
       </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>Data/images/130498.png</t>
+        </is>
+      </c>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
@@ -9188,6 +10198,11 @@
           <t>130499</t>
         </is>
       </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>Data/images/130499.png</t>
+        </is>
+      </c>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
@@ -9195,6 +10210,11 @@
           <t>130509</t>
         </is>
       </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>Data/images/130509.png</t>
+        </is>
+      </c>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
@@ -9202,6 +10222,11 @@
           <t>130510</t>
         </is>
       </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>Data/images/130510.png</t>
+        </is>
+      </c>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
@@ -9209,6 +10234,11 @@
           <t>130511</t>
         </is>
       </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>Data/images/130511.png</t>
+        </is>
+      </c>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
@@ -9216,6 +10246,11 @@
           <t>130518</t>
         </is>
       </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>Data/images/130518.png</t>
+        </is>
+      </c>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
@@ -9223,6 +10258,11 @@
           <t>130521</t>
         </is>
       </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>Data/images/130521.png</t>
+        </is>
+      </c>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
@@ -9230,6 +10270,11 @@
           <t>130523</t>
         </is>
       </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>Data/images/130523.png</t>
+        </is>
+      </c>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
@@ -9297,6 +10342,11 @@
           <t>130537</t>
         </is>
       </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>Data/images/130537.png</t>
+        </is>
+      </c>
     </row>
     <row r="317">
       <c r="A317" t="inlineStr">
@@ -9304,6 +10354,11 @@
           <t>130538</t>
         </is>
       </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>Data/images/130538.png</t>
+        </is>
+      </c>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
@@ -9311,6 +10366,11 @@
           <t>130542</t>
         </is>
       </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>Data/images/130542.png</t>
+        </is>
+      </c>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
@@ -9366,6 +10426,11 @@
           <t>130556</t>
         </is>
       </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>Data/images/130556.png</t>
+        </is>
+      </c>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
@@ -9373,6 +10438,11 @@
           <t>130557</t>
         </is>
       </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>Data/images/130557.png</t>
+        </is>
+      </c>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
@@ -9404,6 +10474,11 @@
           <t>130562</t>
         </is>
       </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>Data/images/130562.png</t>
+        </is>
+      </c>
     </row>
     <row r="328">
       <c r="A328" t="inlineStr">
@@ -9411,6 +10486,11 @@
           <t>130563</t>
         </is>
       </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>Data/images/130563.png</t>
+        </is>
+      </c>
     </row>
     <row r="329">
       <c r="A329" t="inlineStr">
@@ -9418,6 +10498,11 @@
           <t>130569</t>
         </is>
       </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>Data/images/130569.png</t>
+        </is>
+      </c>
     </row>
     <row r="330">
       <c r="A330" t="inlineStr">
@@ -9473,6 +10558,11 @@
           <t>130578</t>
         </is>
       </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>Data/images/130578.png</t>
+        </is>
+      </c>
     </row>
     <row r="335">
       <c r="A335" t="inlineStr">
@@ -9480,6 +10570,11 @@
           <t>130587</t>
         </is>
       </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>Data/images/130587.png</t>
+        </is>
+      </c>
     </row>
     <row r="336">
       <c r="A336" t="inlineStr">
@@ -9487,6 +10582,11 @@
           <t>130591</t>
         </is>
       </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>Data/images/130591.png</t>
+        </is>
+      </c>
     </row>
     <row r="337">
       <c r="A337" t="inlineStr">
@@ -9494,6 +10594,11 @@
           <t>130599</t>
         </is>
       </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>Data/images/130599.png</t>
+        </is>
+      </c>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
@@ -9513,6 +10618,11 @@
           <t>130607</t>
         </is>
       </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>Data/images/130607.png</t>
+        </is>
+      </c>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
@@ -9520,6 +10630,11 @@
           <t>130610</t>
         </is>
       </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>Data/images/130610.png</t>
+        </is>
+      </c>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
@@ -9527,6 +10642,11 @@
           <t>130611</t>
         </is>
       </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>Data/images/130611.png</t>
+        </is>
+      </c>
     </row>
     <row r="342">
       <c r="A342" t="inlineStr">
@@ -9570,6 +10690,11 @@
           <t>130631</t>
         </is>
       </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>Data/images/130631.png</t>
+        </is>
+      </c>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
@@ -9577,6 +10702,11 @@
           <t>130632</t>
         </is>
       </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>Data/images/130632.png</t>
+        </is>
+      </c>
     </row>
     <row r="347">
       <c r="A347" t="inlineStr">
@@ -9584,6 +10714,11 @@
           <t>130642</t>
         </is>
       </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>Data/images/130642.png</t>
+        </is>
+      </c>
     </row>
     <row r="348">
       <c r="A348" t="inlineStr">
@@ -9591,6 +10726,11 @@
           <t>130643</t>
         </is>
       </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>Data/images/130643.png</t>
+        </is>
+      </c>
     </row>
     <row r="349">
       <c r="A349" t="inlineStr">
@@ -9598,6 +10738,11 @@
           <t>130644</t>
         </is>
       </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>Data/images/130644.png</t>
+        </is>
+      </c>
     </row>
     <row r="350">
       <c r="A350" t="inlineStr">
@@ -9725,6 +10870,11 @@
           <t>130710</t>
         </is>
       </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>Data/images/130710.png</t>
+        </is>
+      </c>
     </row>
     <row r="361">
       <c r="A361" t="inlineStr">
@@ -9732,6 +10882,11 @@
           <t>130711</t>
         </is>
       </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>Data/images/130711.png</t>
+        </is>
+      </c>
     </row>
     <row r="362">
       <c r="A362" t="inlineStr">
@@ -9739,6 +10894,11 @@
           <t>130712</t>
         </is>
       </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>Data/images/130712.png</t>
+        </is>
+      </c>
     </row>
     <row r="363">
       <c r="A363" t="inlineStr">
@@ -9794,6 +10954,11 @@
           <t>130731</t>
         </is>
       </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>Data/images/130731.png</t>
+        </is>
+      </c>
     </row>
     <row r="368">
       <c r="A368" t="inlineStr">
@@ -9801,6 +10966,11 @@
           <t>130732</t>
         </is>
       </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>Data/images/130732.png</t>
+        </is>
+      </c>
     </row>
     <row r="369">
       <c r="A369" t="inlineStr">
@@ -9808,6 +10978,11 @@
           <t>130733</t>
         </is>
       </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>Data/images/130733.png</t>
+        </is>
+      </c>
     </row>
     <row r="370">
       <c r="A370" t="inlineStr">
@@ -9815,6 +10990,11 @@
           <t>130734</t>
         </is>
       </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>Data/images/130734.png</t>
+        </is>
+      </c>
     </row>
     <row r="371">
       <c r="A371" t="inlineStr">
@@ -9822,6 +11002,11 @@
           <t>130766</t>
         </is>
       </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>Data/images/130766.png</t>
+        </is>
+      </c>
     </row>
     <row r="372">
       <c r="A372" t="inlineStr">
@@ -9829,6 +11014,11 @@
           <t>130773</t>
         </is>
       </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>Data/images/130773.png</t>
+        </is>
+      </c>
     </row>
     <row r="373">
       <c r="A373" t="inlineStr">
@@ -9848,6 +11038,11 @@
           <t>130782</t>
         </is>
       </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>Data/images/130782.png</t>
+        </is>
+      </c>
     </row>
     <row r="375">
       <c r="A375" t="inlineStr">
@@ -9855,6 +11050,11 @@
           <t>130795</t>
         </is>
       </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>Data/images/130795.png</t>
+        </is>
+      </c>
     </row>
     <row r="376">
       <c r="A376" t="inlineStr">
@@ -9910,6 +11110,11 @@
           <t>130862</t>
         </is>
       </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>Data/images/130862.png</t>
+        </is>
+      </c>
     </row>
     <row r="381">
       <c r="A381" t="inlineStr">
@@ -9917,6 +11122,11 @@
           <t>130886</t>
         </is>
       </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>Data/images/130886.png</t>
+        </is>
+      </c>
     </row>
     <row r="382">
       <c r="A382" t="inlineStr">
@@ -9924,6 +11134,11 @@
           <t>130907</t>
         </is>
       </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>Data/images/130907.png</t>
+        </is>
+      </c>
     </row>
     <row r="383">
       <c r="A383" t="inlineStr">
@@ -9931,6 +11146,11 @@
           <t>89565</t>
         </is>
       </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>Data/images/89565.png</t>
+        </is>
+      </c>
     </row>
     <row r="384">
       <c r="A384" t="inlineStr">
@@ -9938,11 +11158,21 @@
           <t>89566</t>
         </is>
       </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>Data/images/89566.png</t>
+        </is>
+      </c>
     </row>
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
           <t>119510</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>Data/images/119510.png</t>
         </is>
       </c>
     </row>

</xml_diff>